<commit_message>
min-eV PCBv1.2.2 better diode and mosfet footprints, corrected PCBway BOM (OD90 and OD135 resistors were swapped)
</commit_message>
<xml_diff>
--- a/min-eVOLVER/min-eV-PCB/bom/BOM_PCBWay.xlsx
+++ b/min-eVOLVER/min-eV-PCB/bom/BOM_PCBWay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nb\Dropbox\PC\Desktop\share\min-eV-hardware1.2\hardware\Accessories\min-evolver\min-eV-PCB\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nb\Dropbox\PC\Desktop\share\git\min-hardware\hardware\min-eVOLVER\min-eV-PCB\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B080DE9-5936-47F3-B441-F1E8F53A29EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6367A6-B624-4EAD-BF11-C42AE16B06AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20640" yWindow="-17280" windowWidth="20640" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3264" yWindow="-15708" windowWidth="17280" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,6 +432,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -444,7 +445,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -801,7 +801,7 @@
   <dimension ref="A2:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -819,25 +819,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="D2" s="12" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="D2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" customHeight="1">
       <c r="A6" s="3" t="s">
@@ -949,10 +949,10 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>60</v>
@@ -972,10 +972,10 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>60</v>
@@ -1214,32 +1214,32 @@
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" ht="14.4">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" spans="1:9" ht="14.4">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" spans="1:9" ht="14.4">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" spans="1:9" ht="14.1">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
     </row>
     <row r="26" spans="1:9" s="2" customFormat="1" ht="14.1">
       <c r="A26" s="9"/>
@@ -1253,17 +1253,17 @@
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9" ht="14.1">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>